<commit_message>
add duplicate modeling notebook with comprehensive feature selection analysis and chi-squared statistical tests
</commit_message>
<xml_diff>
--- a/prediction_history.xlsx
+++ b/prediction_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -703,6 +703,386 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-11-25 02:45:24.994859</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$9,450.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-11-25 02:46:55.004932</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$9,450.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-11-25 02:47:34.308052</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$9,450.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-11-22 02:49:59.295945</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$150,000.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-11-15 02:53:52.912504</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$1,000,000.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-24 02:56:55.767512</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2156</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$9,500.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.23%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-24 02:57:05.429107</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2156</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$9,500.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.23%</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2022-11-24 02:58:56.682773</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2156</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$9,500.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.13%</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2022-11-25 03:00:51.456492</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2156</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$9,500.00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.19%</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11-25 03:08:44.898061</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>800072000</v>
+      </c>
+      <c r="C17" t="n">
+        <v>100428660</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$9,450.00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>UK Pound</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>ACH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.08%</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>LOW RISK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>